<commit_message>
5,6 menupont + mas kis dolgok
</commit_message>
<xml_diff>
--- a/an_kutyalista.xlsx
+++ b/an_kutyalista.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IKT_projektmunka_LB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Programozás\IKT projekt munka Bandi Lorin\IKT_projektmunka_LB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4404584B-BC7F-40B9-9430-594E6CC4A469}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C89D5B0-A6A0-47FA-B1A6-5F14FAED9A97}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11775" xr2:uid="{0E43BA54-C850-45B2-8E0A-09A15BB270E6}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="64">
   <si>
     <t>Málna</t>
   </si>
@@ -127,6 +127,96 @@
   </si>
   <si>
     <t>szetter</t>
+  </si>
+  <si>
+    <t>Bundás</t>
+  </si>
+  <si>
+    <t>labrador</t>
+  </si>
+  <si>
+    <t>Szuszu</t>
+  </si>
+  <si>
+    <t>csivava</t>
+  </si>
+  <si>
+    <t>Karcsi</t>
+  </si>
+  <si>
+    <t>pitbull</t>
+  </si>
+  <si>
+    <t>Don</t>
+  </si>
+  <si>
+    <t>keverék</t>
+  </si>
+  <si>
+    <t>Dunya</t>
+  </si>
+  <si>
+    <t>németjuhász</t>
+  </si>
+  <si>
+    <t>Lüszi</t>
+  </si>
+  <si>
+    <t>kaukázusi juhászkutya</t>
+  </si>
+  <si>
+    <t>Honey</t>
+  </si>
+  <si>
+    <t>Amy</t>
+  </si>
+  <si>
+    <t>rottweiler</t>
+  </si>
+  <si>
+    <t>Beni</t>
+  </si>
+  <si>
+    <t>Bianka</t>
+  </si>
+  <si>
+    <t>Artúr</t>
+  </si>
+  <si>
+    <t>tacskó</t>
+  </si>
+  <si>
+    <t>Gino</t>
+  </si>
+  <si>
+    <t>juhászkutya</t>
+  </si>
+  <si>
+    <t>Lángos</t>
+  </si>
+  <si>
+    <t>Cserkés</t>
+  </si>
+  <si>
+    <t>Dorisz</t>
+  </si>
+  <si>
+    <t>Cheester</t>
+  </si>
+  <si>
+    <t>staffordshire</t>
+  </si>
+  <si>
+    <t>Artemisz</t>
+  </si>
+  <si>
+    <t>Tyson</t>
+  </si>
+  <si>
+    <t>husky</t>
+  </si>
+  <si>
+    <t>Nudli</t>
   </si>
 </sst>
 </file>
@@ -479,11 +569,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1BDF156-297D-4606-ABF0-E5147D6A7844}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
+      <selection pane="bottomLeft" activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -724,6 +814,443 @@
         <v>26</v>
       </c>
     </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11">
+        <v>2010</v>
+      </c>
+      <c r="C11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12">
+        <v>2016</v>
+      </c>
+      <c r="C12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13">
+        <v>2020</v>
+      </c>
+      <c r="C13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14">
+        <v>2014</v>
+      </c>
+      <c r="C14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15">
+        <v>2018</v>
+      </c>
+      <c r="C15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" t="s">
+        <v>17</v>
+      </c>
+      <c r="G15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16">
+        <v>2021</v>
+      </c>
+      <c r="C16" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17">
+        <v>2020</v>
+      </c>
+      <c r="C17" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" t="s">
+        <v>17</v>
+      </c>
+      <c r="G17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18">
+        <v>2020</v>
+      </c>
+      <c r="C18" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" t="s">
+        <v>17</v>
+      </c>
+      <c r="G18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19">
+        <v>2012</v>
+      </c>
+      <c r="C19" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" t="s">
+        <v>23</v>
+      </c>
+      <c r="E19" t="s">
+        <v>16</v>
+      </c>
+      <c r="F19" t="s">
+        <v>17</v>
+      </c>
+      <c r="G19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20">
+        <v>2011</v>
+      </c>
+      <c r="C20" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" t="s">
+        <v>17</v>
+      </c>
+      <c r="G20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21">
+        <v>2017</v>
+      </c>
+      <c r="C21" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21" t="s">
+        <v>23</v>
+      </c>
+      <c r="E21" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" t="s">
+        <v>17</v>
+      </c>
+      <c r="G21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22">
+        <v>2011</v>
+      </c>
+      <c r="C22" t="s">
+        <v>54</v>
+      </c>
+      <c r="D22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22" t="s">
+        <v>17</v>
+      </c>
+      <c r="G22" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23">
+        <v>2020</v>
+      </c>
+      <c r="C23" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" t="s">
+        <v>16</v>
+      </c>
+      <c r="F23" t="s">
+        <v>17</v>
+      </c>
+      <c r="G23" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>56</v>
+      </c>
+      <c r="B24">
+        <v>2020</v>
+      </c>
+      <c r="C24" t="s">
+        <v>41</v>
+      </c>
+      <c r="D24" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" t="s">
+        <v>16</v>
+      </c>
+      <c r="F24" t="s">
+        <v>17</v>
+      </c>
+      <c r="G24" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>57</v>
+      </c>
+      <c r="B25">
+        <v>2015</v>
+      </c>
+      <c r="C25" t="s">
+        <v>39</v>
+      </c>
+      <c r="D25" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" t="s">
+        <v>11</v>
+      </c>
+      <c r="F25" t="s">
+        <v>17</v>
+      </c>
+      <c r="G25" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26">
+        <v>2018</v>
+      </c>
+      <c r="C26" t="s">
+        <v>59</v>
+      </c>
+      <c r="D26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F26" t="s">
+        <v>17</v>
+      </c>
+      <c r="G26" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>60</v>
+      </c>
+      <c r="B27">
+        <v>2020</v>
+      </c>
+      <c r="C27" t="s">
+        <v>45</v>
+      </c>
+      <c r="D27" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" t="s">
+        <v>11</v>
+      </c>
+      <c r="F27" t="s">
+        <v>17</v>
+      </c>
+      <c r="G27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>61</v>
+      </c>
+      <c r="B28">
+        <v>2022</v>
+      </c>
+      <c r="C28" t="s">
+        <v>62</v>
+      </c>
+      <c r="D28" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28" t="s">
+        <v>16</v>
+      </c>
+      <c r="F28" t="s">
+        <v>5</v>
+      </c>
+      <c r="G28" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>63</v>
+      </c>
+      <c r="B29">
+        <v>2017</v>
+      </c>
+      <c r="C29" t="s">
+        <v>52</v>
+      </c>
+      <c r="D29" t="s">
+        <v>15</v>
+      </c>
+      <c r="E29" t="s">
+        <v>16</v>
+      </c>
+      <c r="F29" t="s">
+        <v>17</v>
+      </c>
+      <c r="G29" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>